<commit_message>
Make Excel Reader & Make new SO, SO Folders & Make Sword
</commit_message>
<xml_diff>
--- a/VampireSurvivalLike/Assets/06 Excels/TBG_Sheet 250224.xlsx
+++ b/VampireSurvivalLike/Assets/06 Excels/TBG_Sheet 250224.xlsx
@@ -2538,8 +2538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE386"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.63000000" defaultRowHeight="15.750000" customHeight="1"/>

</xml_diff>